<commit_message>
completed Generate Excel method, script now fully functional
</commit_message>
<xml_diff>
--- a/testfiles/merged.xlsx
+++ b/testfiles/merged.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernd\Downloads\Csharp\_EXCEL_ExcelAllLanguagesCommonDenominator\testfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60C0B25A-C560-46B0-9033-300881C08135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45E5026E-391F-469C-B7BC-401AB6B4B643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="810" windowWidth="10290" windowHeight="8325" xr2:uid="{6CF8EEE5-09D4-4B8F-BA19-89AC79904A70}"/>
+    <workbookView xWindow="9840" yWindow="810" windowWidth="10290" windowHeight="8325" xr2:uid="{559AC4F5-06DE-4AE6-AA5E-3B7A34C274B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Source language</t>
   </si>
@@ -45,6 +45,24 @@
   </si>
   <si>
     <t>Target language 2</t>
+  </si>
+  <si>
+    <t>The cat is on the roof.</t>
+  </si>
+  <si>
+    <t>Die Katze ist auf dem Dach.</t>
+  </si>
+  <si>
+    <t>Katten är på taket.</t>
+  </si>
+  <si>
+    <t>Signal improvement</t>
+  </si>
+  <si>
+    <t>Signalverbesserung</t>
+  </si>
+  <si>
+    <t>Signalförbättring</t>
   </si>
 </sst>
 </file>
@@ -415,8 +433,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5E13E6-614C-4D24-89F2-7CA8279D303A}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A3C5C3-58DF-4E27-866A-7E2112775A5A}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -433,6 +451,28 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>